<commit_message>
moar stuff on lab 3
</commit_message>
<xml_diff>
--- a/lab3/tabelas/tabelas comando conversor.xlsx
+++ b/lab3/tabelas/tabelas comando conversor.xlsx
@@ -22,7 +22,7 @@
     <t>Vo experimental [V]</t>
   </si>
   <si>
-    <t xml:space="preserve"> Ângulo de Disparo - α [º]</t>
+    <t>Fator de ciclo, D</t>
   </si>
 </sst>
 </file>
@@ -56,7 +56,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -151,19 +151,6 @@
       </top>
       <bottom style="thin">
         <color theme="3"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -187,19 +174,6 @@
       <right style="thin">
         <color theme="0"/>
       </right>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0"/>
-      </left>
-      <right style="thin">
-        <color theme="0"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color theme="0"/>
@@ -273,19 +247,17 @@
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -298,13 +270,17 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -337,44 +313,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="pt-PT"/>
-              <a:t>Tensão na carga em função do</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-PT" baseline="0"/>
-              <a:t> Ângulo de Disparo </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="el-GR" baseline="0"/>
-              <a:t>α</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="pt-PT" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:endParaRPr lang="pt-PT"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -408,8 +346,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -426,7 +364,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -435,62 +373,68 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$9</c:f>
+              <c:f>'5.2.f'!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'5.2.f'!$E$4:$E$9</c:f>
+              <c:f>'5.2.f'!$E$4:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15.915494309189533</c:v>
+                  <c:v>15.644340650296199</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14.849358347367168</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.93662073189215</c:v>
+                  <c:v>13.072888426586596</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.9577471545947667</c:v>
+                  <c:v>10.679456976958702</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9788735772973851</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.0661359618223656</c:v>
+                  <c:v>8.6513105184515364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:ser>
@@ -508,7 +452,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -517,62 +461,68 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:cat>
+          <c:xVal>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$9</c:f>
+              <c:f>'5.2.f'!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>60</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>90</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>150</c:v>
+                  <c:v>85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>'5.2.f'!$F$4:$F$9</c:f>
+              <c:f>'5.2.f'!$F$4:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>14.5</c:v>
+                  <c:v>2.58</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.35</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>13.2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.22</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.08</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.15</c:v>
+                  <c:v>16.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
@@ -583,17 +533,30 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="216276360"/>
-        <c:axId val="216138472"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="216276360"/>
+        <c:axId val="499207232"/>
+        <c:axId val="499206840"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="499207232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -603,8 +566,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -631,15 +594,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216138472"/>
+        <c:crossAx val="499206840"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="216138472"/>
+        <c:axId val="499206840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -665,8 +625,14 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -690,9 +656,9 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216276360"/>
+        <c:crossAx val="499207232"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -812,7 +778,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -839,8 +805,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -920,11 +886,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -935,11 +896,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -951,7 +907,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -971,9 +927,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -986,10 +939,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1029,22 +982,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1149,8 +1103,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1282,19 +1236,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1308,6 +1263,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -1332,19 +1298,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
+      <xdr:colOff>110712</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:rowOff>37356</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>219074</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>467591</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155863</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1651,25 +1617,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="3"/>
-    <col min="4" max="4" width="23.85546875" style="3" customWidth="1"/>
-    <col min="5" max="6" width="22.7109375" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="6"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1681,18 +1647,18 @@
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="1"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1704,19 +1670,19 @@
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C4" s="4"/>
-      <c r="D4" s="9">
-        <v>0</v>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7">
+        <v>15</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="8">
         <f>(50/(2*PI())*(1+COS(D4*PI()/180)))</f>
-        <v>15.915494309189533</v>
+        <v>15.644340650296199</v>
       </c>
-      <c r="F4" s="11">
-        <v>14.5</v>
+      <c r="F4" s="9">
+        <v>2.58</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="1"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1728,19 +1694,19 @@
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C5" s="4"/>
-      <c r="D5" s="9">
+      <c r="C5" s="14"/>
+      <c r="D5" s="7">
         <v>30</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <f t="shared" ref="E5:E9" si="0">(50/(2*PI())*(1+COS(D5*PI()/180)))</f>
         <v>14.849358347367168</v>
       </c>
-      <c r="F5" s="11">
-        <v>13.2</v>
+      <c r="F5" s="9">
+        <v>5.25</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="1"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="6"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1752,19 +1718,19 @@
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C6" s="4"/>
-      <c r="D6" s="9">
-        <v>60</v>
+      <c r="C6" s="14"/>
+      <c r="D6" s="7">
+        <v>50</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="8">
         <f t="shared" si="0"/>
-        <v>11.93662073189215</v>
+        <v>13.072888426586596</v>
       </c>
-      <c r="F6" s="11">
-        <v>11</v>
+      <c r="F6" s="9">
+        <v>9.35</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="1"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1776,19 +1742,19 @@
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C7" s="4"/>
-      <c r="D7" s="9">
-        <v>90</v>
+      <c r="C7" s="14"/>
+      <c r="D7" s="7">
+        <v>70</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>7.9577471545947667</v>
+        <v>10.679456976958702</v>
       </c>
-      <c r="F7" s="11">
-        <v>6.22</v>
+      <c r="F7" s="9">
+        <v>13.2</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="1"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1799,20 +1765,20 @@
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
     </row>
-    <row r="8" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
-      <c r="D8" s="9">
-        <v>120</v>
+    <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C8" s="14"/>
+      <c r="D8" s="10">
+        <v>85</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>3.9788735772973851</v>
+        <v>8.6513105184515364</v>
       </c>
-      <c r="F8" s="11">
-        <v>2.08</v>
+      <c r="F8" s="12">
+        <v>16.2</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="1"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1823,20 +1789,13 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="4"/>
-      <c r="D9" s="12">
-        <v>150</v>
-      </c>
-      <c r="E9" s="13">
-        <f t="shared" si="0"/>
-        <v>1.0661359618223656</v>
-      </c>
-      <c r="F9" s="14">
-        <v>0.15</v>
-      </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="1"/>
+    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1848,12 +1807,12 @@
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="1"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="6"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1865,11 +1824,11 @@
       <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>

</xml_diff>

<commit_message>
lab 3: buck maybe done
</commit_message>
<xml_diff>
--- a/lab3/tabelas/tabelas comando conversor.xlsx
+++ b/lab3/tabelas/tabelas comando conversor.xlsx
@@ -56,7 +56,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -237,6 +237,32 @@
       </top>
       <bottom style="medium">
         <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0"/>
       </bottom>
       <diagonal/>
     </border>
@@ -276,9 +302,9 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -313,6 +339,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Tensão</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> de Saída, Vo, em função do fator de ciclo, D</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -394,19 +450,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,19 +474,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15.644340650296199</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.849358347367168</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.072888426586596</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.679456976958702</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6513105184515364</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -482,19 +538,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>70</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>85</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -533,11 +589,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="499207232"/>
-        <c:axId val="499206840"/>
+        <c:axId val="216606888"/>
+        <c:axId val="72658128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="499207232"/>
+        <c:axId val="216606888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -557,6 +613,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fator</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de ciclo, D</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -594,12 +711,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499206840"/>
+        <c:crossAx val="72658128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="499206840"/>
+        <c:axId val="72658128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -619,6 +736,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tensão de Saída, Vo [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -656,7 +829,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="499207232"/>
+        <c:crossAx val="216606888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1298,15 +1471,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>110712</xdr:colOff>
+      <xdr:colOff>144330</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>37356</xdr:rowOff>
+      <xdr:rowOff>14944</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>467591</xdr:colOff>
+      <xdr:colOff>501209</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>155863</xdr:rowOff>
+      <xdr:rowOff>133451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1615,10 +1788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:Q21"/>
+  <dimension ref="B1:W27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1629,13 +1802,38 @@
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="6"/>
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1645,8 +1843,15 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
       <c r="C3" s="14"/>
       <c r="D3" s="3" t="s">
         <v>2</v>
@@ -1657,8 +1862,8 @@
       <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -1668,21 +1873,28 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
       <c r="C4" s="14"/>
       <c r="D4" s="7">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="E4" s="8">
-        <f>(50/(2*PI())*(1+COS(D4*PI()/180)))</f>
-        <v>15.644340650296199</v>
+        <f>D4*20</f>
+        <v>3</v>
       </c>
       <c r="F4" s="9">
         <v>2.58</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -1692,21 +1904,28 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
       <c r="C5" s="14"/>
       <c r="D5" s="7">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="E5" s="8">
-        <f t="shared" ref="E5:E9" si="0">(50/(2*PI())*(1+COS(D5*PI()/180)))</f>
-        <v>14.849358347367168</v>
+        <f t="shared" ref="E5:E8" si="0">D5*20</f>
+        <v>6</v>
       </c>
       <c r="F5" s="9">
         <v>5.25</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -1716,21 +1935,28 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
       <c r="C6" s="14"/>
       <c r="D6" s="7">
-        <v>50</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="8">
         <f t="shared" si="0"/>
-        <v>13.072888426586596</v>
+        <v>10</v>
       </c>
       <c r="F6" s="9">
         <v>9.35</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1740,21 +1966,28 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
       <c r="C7" s="14"/>
       <c r="D7" s="7">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="E7" s="8">
         <f t="shared" si="0"/>
-        <v>10.679456976958702</v>
+        <v>14</v>
       </c>
       <c r="F7" s="9">
         <v>13.2</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -1764,21 +1997,28 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1"/>
-    </row>
-    <row r="8" spans="3:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
       <c r="C8" s="14"/>
       <c r="D8" s="10">
-        <v>85</v>
+        <v>0.85</v>
       </c>
       <c r="E8" s="11">
         <f t="shared" si="0"/>
-        <v>8.6513105184515364</v>
+        <v>17</v>
       </c>
       <c r="F8" s="12">
         <v>16.2</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -1788,14 +2028,21 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C9" s="14"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="6"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -1805,14 +2052,21 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="6"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -1822,13 +2076,20 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
-    </row>
-    <row r="11" spans="3:17" x14ac:dyDescent="0.25">
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1839,8 +2100,15 @@
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -1856,8 +2124,15 @@
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
-    </row>
-    <row r="13" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1873,8 +2148,15 @@
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1890,8 +2172,15 @@
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
-    </row>
-    <row r="15" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1907,8 +2196,15 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
-    </row>
-    <row r="16" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1924,8 +2220,15 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
-    </row>
-    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -1941,8 +2244,15 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-    </row>
-    <row r="18" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -1958,8 +2268,15 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-    </row>
-    <row r="19" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -1975,8 +2292,15 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
-    </row>
-    <row r="20" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -1992,8 +2316,15 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -2009,6 +2340,156 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lab 3: is it done?
</commit_message>
<xml_diff>
--- a/lab3/tabelas/tabelas comando conversor.xlsx
+++ b/lab3/tabelas/tabelas comando conversor.xlsx
@@ -4,17 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="5.2.f" sheetId="1" r:id="rId1"/>
+    <sheet name="Buck" sheetId="1" r:id="rId1"/>
+    <sheet name="Boost" sheetId="2" r:id="rId2"/>
+    <sheet name="Buck-boost" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
   <si>
     <t>Vo teórico [V]</t>
   </si>
@@ -270,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,6 +309,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,7 +413,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5.2.f'!$E$3</c:f>
+              <c:f>Buck!$E$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -445,7 +448,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$8</c:f>
+              <c:f>Buck!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -469,7 +472,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5.2.f'!$E$4:$E$8</c:f>
+              <c:f>Buck!$E$4:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -498,7 +501,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'5.2.f'!$F$3</c:f>
+              <c:f>Buck!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -533,7 +536,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'5.2.f'!$D$4:$D$8</c:f>
+              <c:f>Buck!$D$4:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -557,7 +560,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'5.2.f'!$F$4:$F$8</c:f>
+              <c:f>Buck!$F$4:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
@@ -589,11 +592,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="216606888"/>
-        <c:axId val="72658128"/>
+        <c:axId val="185906456"/>
+        <c:axId val="216476576"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="216606888"/>
+        <c:axId val="185906456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -711,12 +714,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="72658128"/>
+        <c:crossAx val="216476576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="72658128"/>
+        <c:axId val="216476576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -829,7 +832,1155 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="216606888"/>
+        <c:crossAx val="185906456"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Tensão</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> de Saída, Vo, em função do fator de ciclo, D</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Boost!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo teórico [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Boost!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Boost!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>11.764705882352942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.666666666666668</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Boost!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo experimental [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Boost!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Boost!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="503213944"/>
+        <c:axId val="503211592"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="503213944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fator</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de ciclo, D</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503211592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="503211592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tensão de Saída, Vo [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503213944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Tensão</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="pt-PT" baseline="0"/>
+              <a:t> de Saída, Vo, em função do fator de ciclo, D</a:t>
+            </a:r>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Buck-boost'!$E$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo teórico [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Buck-boost'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Buck-boost'!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-1.7647058823529411</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-4.2857142857142856</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Buck-boost'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vo experimental [V]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Buck-boost'!$D$4:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Buck-boost'!$F$4:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>-2.04</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.09</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-9.7100000000000009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-16.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="549747896"/>
+        <c:axId val="549748288"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="549747896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Fator</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> de ciclo, D</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549748288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="549748288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Tensão de Saída, Vo [V]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="549747896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -950,7 +2101,1119 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1485,6 +3748,80 @@
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Gráfico 2"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>144330</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14944</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>501209</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133451</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>144330</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14944</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>501209</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133451</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1790,8 +4127,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,4 +4833,1412 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:W27"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="8">
+        <f>10/(1-D4)</f>
+        <v>11.764705882352942</v>
+      </c>
+      <c r="F4" s="9">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" ref="E5:E7" si="0">10/(1-D5)</f>
+        <v>12.5</v>
+      </c>
+      <c r="F5" s="9">
+        <v>10.9</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="E6" s="8">
+        <f t="shared" si="0"/>
+        <v>14.285714285714286</v>
+      </c>
+      <c r="F6" s="9">
+        <v>12.3</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="F7" s="12">
+        <v>14.3</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:W27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="23.85546875" style="2" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+    </row>
+    <row r="2" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" s="1"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="E4" s="8">
+        <f>-(10*D4)/(1-D4)</f>
+        <v>-1.7647058823529411</v>
+      </c>
+      <c r="F4" s="9">
+        <v>-2.04</v>
+      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="E5" s="8">
+        <f>-(10*D5)/(1-D5)</f>
+        <v>-4.2857142857142856</v>
+      </c>
+      <c r="F5" s="9">
+        <v>-5.09</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="E6" s="8">
+        <f>-(10*D6)/(1-D6)</f>
+        <v>-10</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-9.7100000000000009</v>
+      </c>
+      <c r="G6" s="6"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+    </row>
+    <row r="7" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="E7" s="11">
+        <f>-(10*D7)/(1-D7)</f>
+        <v>-15</v>
+      </c>
+      <c r="F7" s="12">
+        <v>-16.2</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+    </row>
+    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+    </row>
+    <row r="14" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+    </row>
+    <row r="15" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+    </row>
+    <row r="16" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>